<commit_message>
Actualizacion de lab 1
</commit_message>
<xml_diff>
--- a/Lab1_Procesos/datos_mediciones_lab1.xlsx
+++ b/Lab1_Procesos/datos_mediciones_lab1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\under\OneDrive\Documentos\Laboratorio_SO_Guillermo_Zorrilla\Lab1_Procesos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B3D485B5-DC95-41E3-8ECA-DC7BB5439031}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42A7B87F-7BC2-4EB7-8525-F21069C7C2A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="22">
   <si>
     <t>Estado Inicial</t>
   </si>
@@ -68,6 +68,24 @@
   </si>
   <si>
     <t xml:space="preserve">Esto fue del deadlock simulado </t>
+  </si>
+  <si>
+    <t>Proceso ID</t>
+  </si>
+  <si>
+    <t>Tipo de Transición</t>
+  </si>
+  <si>
+    <t>Tiempo (ms)</t>
+  </si>
+  <si>
+    <t>Ready → Running</t>
+  </si>
+  <si>
+    <t>Tiempo promedio</t>
+  </si>
+  <si>
+    <t>Esto fue de simulacion para la Medir tiempos de transición entre estado</t>
   </si>
 </sst>
 </file>
@@ -109,7 +127,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -141,19 +159,168 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -460,10 +627,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -491,68 +658,68 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="5">
         <v>2</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="6" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="8">
         <v>2</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="9" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="8">
         <v>1.5</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="9" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="11">
         <v>2</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="12" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
+      <c r="B6" s="22"/>
+      <c r="C6" s="22"/>
+      <c r="D6" s="23"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
@@ -569,22 +736,106 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="A8" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="13" t="s">
         <v>14</v>
       </c>
     </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="19"/>
+      <c r="C9" s="19"/>
+      <c r="D9" s="20"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="17" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="4">
+        <v>1</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="14">
+        <v>1661</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="7">
+        <v>2</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" s="15">
+        <v>4720</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="7">
+        <v>3</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" s="15">
+        <v>3023</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="7">
+        <v>4</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14" s="15">
+        <v>2038</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="7">
+        <v>5</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" s="15">
+        <v>1680</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="10"/>
+      <c r="B16" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" s="16">
+        <v>2624</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="A6:D6"/>
+    <mergeCell ref="A9:D9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>